<commit_message>
added wilcoxon, friedman, posthoc and visualisation. survival curves, logistic regression and ROC visualisation next
</commit_message>
<xml_diff>
--- a/results/descriptive_statistics.xlsx
+++ b/results/descriptive_statistics.xlsx
@@ -617,19 +617,19 @@
         <v>2798</v>
       </c>
       <c r="D4" t="n">
-        <v>26.41956413004829</v>
+        <v>26.05193919343433</v>
       </c>
       <c r="E4" t="n">
-        <v>15.51650573971546</v>
+        <v>15.29439420494566</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.9497446270443026</v>
       </c>
       <c r="G4" t="n">
-        <v>17.61993510736059</v>
+        <v>17</v>
       </c>
       <c r="H4" t="n">
-        <v>22.95375715481205</v>
+        <v>22.16989285697366</v>
       </c>
       <c r="I4" t="n">
         <v>30</v>
@@ -638,10 +638,10 @@
         <v>182</v>
       </c>
       <c r="K4" t="n">
-        <v>3.011866768321068</v>
+        <v>3.043281450982875</v>
       </c>
       <c r="L4" t="n">
-        <v>16.91649525611243</v>
+        <v>17.47739465223725</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>

</xml_diff>